<commit_message>
DAWN NWBO PM and others
</commit_message>
<xml_diff>
--- a/Alzheimer's.xlsx
+++ b/Alzheimer's.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6446F4-18FC-4E8C-B3CE-6C58E6C8C3EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115A007C-A2FA-412C-A095-C881383AB0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34860" yWindow="1020" windowWidth="32100" windowHeight="19275" firstSheet="1" activeTab="1" xr2:uid="{3DB1B341-C349-45CE-8B3C-A48AF4C5DB82}"/>
+    <workbookView xWindow="-29685" yWindow="2850" windowWidth="28305" windowHeight="17085" firstSheet="1" activeTab="3" xr2:uid="{3DB1B341-C349-45CE-8B3C-A48AF4C5DB82}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Adas-Cog Raw" sheetId="13" r:id="rId2"/>
-    <sheet name="Drugs" sheetId="2" r:id="rId3"/>
-    <sheet name="verubecestat" sheetId="12" r:id="rId4"/>
-    <sheet name="Literature" sheetId="3" r:id="rId5"/>
+    <sheet name="Literature" sheetId="3" r:id="rId3"/>
+    <sheet name="Drugs" sheetId="2" r:id="rId4"/>
+    <sheet name="verubecestat" sheetId="12" r:id="rId5"/>
     <sheet name="donanemab" sheetId="4" r:id="rId6"/>
     <sheet name="bapi" sheetId="5" r:id="rId7"/>
     <sheet name="lecanemab" sheetId="6" r:id="rId8"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2829" uniqueCount="2574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2836" uniqueCount="2580">
   <si>
     <t>Name</t>
   </si>
@@ -7797,6 +7797,24 @@
   </si>
   <si>
     <t>https://pubmed.ncbi.nlm.nih.gov/38849944/</t>
+  </si>
+  <si>
+    <t>ADAS-Cog13 (0-85)</t>
+  </si>
+  <si>
+    <t>28.7-29.3</t>
+  </si>
+  <si>
+    <t>28.53 --&gt; 32.72</t>
+  </si>
+  <si>
+    <t>29.16 --&gt; 34.53</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/37459141/</t>
+  </si>
+  <si>
+    <t>1.8 --&gt; 1.3 at 18 months (p&lt;0.001)</t>
   </si>
 </sst>
 </file>
@@ -28121,11 +28139,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{178605DD-42A6-477A-B19E-71CF1B2C86A8}">
   <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H72" sqref="H72"/>
+      <selection pane="bottomRight" activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -29781,11 +29799,36 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFE267D6-BDDE-4A05-88E6-A834CD3AD9C1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="Main!A1" display="Main" xr:uid="{D832545E-69EA-4AE3-81C5-BD2937606728}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D9C21B7-4763-4FF8-84CA-74B3A916DA87}">
-  <dimension ref="A1:L68"/>
+  <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -30486,6 +30529,16 @@
     <row r="68" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>2544</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B70" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B71" t="s">
+        <v>2579</v>
       </c>
     </row>
   </sheetData>
@@ -30512,7 +30565,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53F3AD44-E03D-45FA-9764-4B48B650EA89}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -30549,37 +30602,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFE267D6-BDDE-4A05-88E6-A834CD3AD9C1}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" location="Main!A1" display="Main" xr:uid="{D832545E-69EA-4AE3-81C5-BD2937606728}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F4A264A-38A5-42EE-B7CD-F6096EA00AB2}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="G10" sqref="B10:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -30588,12 +30616,12 @@
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -30601,7 +30629,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -30609,7 +30637,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -30617,7 +30645,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -30625,7 +30653,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>638</v>
       </c>
@@ -30633,34 +30661,79 @@
         <v>639</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C8" s="10" t="s">
         <v>630</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C14" s="10" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>637</v>
+      </c>
+      <c r="G15" t="s">
+        <v>2578</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>2574</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>2575</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>1.33</v>
+      </c>
+      <c r="D18">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>2576</v>
+      </c>
+      <c r="F19">
+        <f>32.72-28.53</f>
+        <v>4.1899999999999977</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>2577</v>
+      </c>
+      <c r="F20">
+        <f>34.53-29.16</f>
+        <v>5.370000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="F21">
+        <f>+F20-F19</f>
+        <v>1.1800000000000033</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated QCOM INTC models
</commit_message>
<xml_diff>
--- a/Alzheimer's.xlsx
+++ b/Alzheimer's.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115A007C-A2FA-412C-A095-C881383AB0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AB6732-4C2C-4B44-AF62-95C304FD67ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29685" yWindow="2850" windowWidth="28305" windowHeight="17085" firstSheet="1" activeTab="3" xr2:uid="{3DB1B341-C349-45CE-8B3C-A48AF4C5DB82}"/>
+    <workbookView xWindow="-50430" yWindow="1170" windowWidth="38700" windowHeight="15345" firstSheet="1" activeTab="3" xr2:uid="{3DB1B341-C349-45CE-8B3C-A48AF4C5DB82}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -29827,8 +29827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D9C21B7-4763-4FF8-84CA-74B3A916DA87}">
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated SAVA, PYPL, CRL, FIVN, ADMA and others
</commit_message>
<xml_diff>
--- a/Alzheimer's.xlsx
+++ b/Alzheimer's.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43E21C7-D4A7-4EE7-820F-F9455F70D81A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8FCCD6-43D5-404F-B355-9475BEA5AABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-39735" yWindow="1005" windowWidth="35220" windowHeight="19110" firstSheet="1" activeTab="3" xr2:uid="{3DB1B341-C349-45CE-8B3C-A48AF4C5DB82}"/>
+    <workbookView xWindow="-44205" yWindow="2475" windowWidth="37305" windowHeight="16920" xr2:uid="{3DB1B341-C349-45CE-8B3C-A48AF4C5DB82}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2836" uniqueCount="2580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2837" uniqueCount="2580">
   <si>
     <t>Name</t>
   </si>
@@ -8474,9 +8474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7835E389-3380-44CD-883B-FD2EDD57702B}">
   <dimension ref="B2:D40"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -28140,10 +28138,10 @@
   <dimension ref="A1:J73"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C54" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B74" sqref="B74"/>
+      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -29800,26 +29798,34 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFE267D6-BDDE-4A05-88E6-A834CD3AD9C1}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B2" s="9" t="s">
+        <v>2556</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" location="Main!A1" display="Main" xr:uid="{D832545E-69EA-4AE3-81C5-BD2937606728}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{10C41B2C-8709-41AB-9CA1-95F6138F6297}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -29827,7 +29833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D9C21B7-4763-4FF8-84CA-74B3A916DA87}">
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
@@ -30607,7 +30613,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="G10" sqref="B10:G11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated INTC, PLTR, created APP
</commit_message>
<xml_diff>
--- a/Alzheimer's.xlsx
+++ b/Alzheimer's.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0BAA511-5FA2-4770-A76F-F1ABB4527E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5EAB9AD-542E-41B6-83C5-C00422252A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33090" yWindow="2910" windowWidth="32820" windowHeight="15960" activeTab="1" xr2:uid="{3DB1B341-C349-45CE-8B3C-A48AF4C5DB82}"/>
+    <workbookView xWindow="-25845" yWindow="2520" windowWidth="25215" windowHeight="16575" activeTab="3" xr2:uid="{3DB1B341-C349-45CE-8B3C-A48AF4C5DB82}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -8228,7 +8228,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -8267,6 +8267,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -30717,11 +30718,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{178605DD-42A6-477A-B19E-71CF1B2C86A8}">
   <dimension ref="A1:O230"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="F28" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F39" sqref="F39"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -37413,8 +37414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D9C21B7-4763-4FF8-84CA-74B3A916DA87}">
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="295" zoomScaleNormal="295" workbookViewId="0">
+      <selection activeCell="C65" sqref="B64:C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -38040,31 +38041,31 @@
       </c>
       <c r="H48" s="5"/>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B49" s="30" t="s">
         <v>2557</v>
       </c>
       <c r="H49" s="5"/>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B50" s="4" t="s">
         <v>548</v>
       </c>
       <c r="H50" s="5"/>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B51" s="4" t="s">
         <v>535</v>
       </c>
       <c r="H51" s="5"/>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B52" s="4" t="s">
         <v>536</v>
       </c>
       <c r="H52" s="5"/>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B53" s="6" t="s">
         <v>524</v>
       </c>
@@ -38075,63 +38076,72 @@
       <c r="G53" s="7"/>
       <c r="H53" s="8"/>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B55" s="10" t="s">
         <v>2534</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>2538</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B58" s="10" t="s">
         <v>2535</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>2537</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B61" s="10" t="s">
         <v>2536</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>2540</v>
       </c>
       <c r="C62" s="25"/>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="26"/>
       <c r="B64" s="10" t="s">
         <v>2539</v>
       </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B65" t="s">
+      <c r="C64" s="26"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="26"/>
+      <c r="B65" s="34" t="s">
         <v>2541</v>
       </c>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C65" s="34"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="26"/>
+      <c r="B66" s="26"/>
+      <c r="C66" s="26"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B67" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>2542</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B70" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>2576</v>
       </c>

</xml_diff>